<commit_message>
Added Caribbean panel data
</commit_message>
<xml_diff>
--- a/data/countries/_CARIBBEAN.xlsx
+++ b/data/countries/_CARIBBEAN.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andreipascu/Documents/Yale University/Years/Senior/Spring/CSEC 491/local/data/countries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548DD45C-A1C5-5542-B6CA-4E04DAC96D2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{550A3578-AB8E-E046-8C12-D0489A210DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="340" yWindow="500" windowWidth="27640" windowHeight="16060" activeTab="1" xr2:uid="{A00892F2-77B1-0143-89C4-5296CC556B66}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
-    <sheet name="Monthly" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2185" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2117" uniqueCount="73">
   <si>
     <t>General</t>
   </si>
@@ -199,9 +198,6 @@
     <t>cuba</t>
   </si>
   <si>
-    <t>mo</t>
-  </si>
-  <si>
     <t>Mo. Volume</t>
   </si>
   <si>
@@ -263,9 +259,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="[$-409]mmm\-yy;@"/>
-  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -364,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -406,7 +399,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -880,7 +872,7 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>7</v>
@@ -902,7 +894,7 @@
         <v>9</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.2">
@@ -910,7 +902,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.2">
@@ -992,9 +984,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7D00AED-5EBD-974C-A23B-D47D16AC0D47}">
   <dimension ref="A1:O313"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A290" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M301" sqref="M301:O313"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L320" sqref="L320"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6035,7 +6027,7 @@
     </row>
     <row r="106" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A106" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B106">
         <v>12.169600000000001</v>
@@ -6084,7 +6076,7 @@
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A107" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B107">
         <v>12.169600000000001</v>
@@ -6133,7 +6125,7 @@
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A108" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B108">
         <v>12.169600000000001</v>
@@ -6182,7 +6174,7 @@
     </row>
     <row r="109" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A109" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B109">
         <v>12.169600000000001</v>
@@ -6231,7 +6223,7 @@
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A110" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B110">
         <v>12.169600000000001</v>
@@ -6280,7 +6272,7 @@
     </row>
     <row r="111" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A111" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B111">
         <v>12.169600000000001</v>
@@ -6329,7 +6321,7 @@
     </row>
     <row r="112" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A112" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B112">
         <v>12.169600000000001</v>
@@ -6378,7 +6370,7 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A113" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B113">
         <v>12.169600000000001</v>
@@ -6427,7 +6419,7 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A114" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B114">
         <v>12.169600000000001</v>
@@ -6476,7 +6468,7 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A115" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B115">
         <v>12.169600000000001</v>
@@ -6525,7 +6517,7 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A116" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B116">
         <v>12.169600000000001</v>
@@ -6575,7 +6567,7 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A117" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B117">
         <v>12.169600000000001</v>
@@ -6624,7 +6616,7 @@
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A118" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B118">
         <v>12.169600000000001</v>
@@ -6672,7 +6664,7 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A119" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B119">
         <v>15.414999999999999</v>
@@ -6719,7 +6711,7 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A120" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B120">
         <v>15.414999999999999</v>
@@ -6766,7 +6758,7 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A121" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B121">
         <v>15.414999999999999</v>
@@ -6813,7 +6805,7 @@
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A122" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B122">
         <v>15.414999999999999</v>
@@ -6860,7 +6852,7 @@
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A123" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B123">
         <v>15.414999999999999</v>
@@ -6907,7 +6899,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A124" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B124">
         <v>15.414999999999999</v>
@@ -6954,7 +6946,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A125" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B125">
         <v>15.414999999999999</v>
@@ -7001,7 +6993,7 @@
     </row>
     <row r="126" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A126" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B126">
         <v>15.414999999999999</v>
@@ -7048,7 +7040,7 @@
     </row>
     <row r="127" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A127" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B127">
         <v>15.414999999999999</v>
@@ -7095,7 +7087,7 @@
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A128" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B128">
         <v>15.414999999999999</v>
@@ -7142,7 +7134,7 @@
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A129" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B129">
         <v>15.414999999999999</v>
@@ -7190,7 +7182,7 @@
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A130" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B130">
         <v>15.414999999999999</v>
@@ -7238,7 +7230,7 @@
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A131" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B131">
         <v>15.414999999999999</v>
@@ -7286,7 +7278,7 @@
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A132" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B132">
         <v>18.735700000000001</v>
@@ -7333,7 +7325,7 @@
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A133" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B133">
         <v>18.735700000000001</v>
@@ -7380,7 +7372,7 @@
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A134" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B134">
         <v>18.735700000000001</v>
@@ -7427,7 +7419,7 @@
     </row>
     <row r="135" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A135" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B135">
         <v>18.735700000000001</v>
@@ -7474,7 +7466,7 @@
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A136" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B136">
         <v>18.735700000000001</v>
@@ -7521,7 +7513,7 @@
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A137" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B137">
         <v>18.735700000000001</v>
@@ -7568,7 +7560,7 @@
     </row>
     <row r="138" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A138" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B138">
         <v>18.735700000000001</v>
@@ -7615,7 +7607,7 @@
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A139" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B139">
         <v>18.735700000000001</v>
@@ -7662,7 +7654,7 @@
     </row>
     <row r="140" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A140" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B140">
         <v>18.735700000000001</v>
@@ -7709,7 +7701,7 @@
     </row>
     <row r="141" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A141" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B141">
         <v>18.735700000000001</v>
@@ -7756,7 +7748,7 @@
     </row>
     <row r="142" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A142" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B142">
         <v>18.735700000000001</v>
@@ -7804,7 +7796,7 @@
     </row>
     <row r="143" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A143" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B143">
         <v>18.735700000000001</v>
@@ -7852,7 +7844,7 @@
     </row>
     <row r="144" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A144" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B144">
         <v>18.735700000000001</v>
@@ -7900,7 +7892,7 @@
     </row>
     <row r="145" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A145" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B145">
         <v>12.1165</v>
@@ -7947,7 +7939,7 @@
     </row>
     <row r="146" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A146" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B146">
         <v>12.1165</v>
@@ -7994,7 +7986,7 @@
     </row>
     <row r="147" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A147" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B147">
         <v>12.1165</v>
@@ -8041,7 +8033,7 @@
     </row>
     <row r="148" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A148" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B148">
         <v>12.1165</v>
@@ -8088,7 +8080,7 @@
     </row>
     <row r="149" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A149" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B149">
         <v>12.1165</v>
@@ -8135,7 +8127,7 @@
     </row>
     <row r="150" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A150" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B150">
         <v>12.1165</v>
@@ -8182,7 +8174,7 @@
     </row>
     <row r="151" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A151" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B151">
         <v>12.1165</v>
@@ -8229,7 +8221,7 @@
     </row>
     <row r="152" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A152" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B152">
         <v>12.1165</v>
@@ -8276,7 +8268,7 @@
     </row>
     <row r="153" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A153" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B153">
         <v>12.1165</v>
@@ -8323,7 +8315,7 @@
     </row>
     <row r="154" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A154" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B154">
         <v>12.1165</v>
@@ -8370,7 +8362,7 @@
     </row>
     <row r="155" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A155" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B155">
         <v>12.1165</v>
@@ -8418,7 +8410,7 @@
     </row>
     <row r="156" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A156" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B156">
         <v>12.1165</v>
@@ -8466,7 +8458,7 @@
     </row>
     <row r="157" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A157" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B157">
         <v>12.1165</v>
@@ -8514,7 +8506,7 @@
     </row>
     <row r="158" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A158" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B158">
         <v>18.9712</v>
@@ -8562,7 +8554,7 @@
     </row>
     <row r="159" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A159" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B159">
         <v>18.9712</v>
@@ -8610,7 +8602,7 @@
     </row>
     <row r="160" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A160" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B160">
         <v>18.9712</v>
@@ -8658,7 +8650,7 @@
     </row>
     <row r="161" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A161" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B161">
         <v>18.9712</v>
@@ -8706,7 +8698,7 @@
     </row>
     <row r="162" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A162" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B162">
         <v>18.9712</v>
@@ -8754,7 +8746,7 @@
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A163" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B163">
         <v>18.9712</v>
@@ -8802,7 +8794,7 @@
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A164" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B164">
         <v>18.9712</v>
@@ -8850,7 +8842,7 @@
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A165" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B165">
         <v>18.9712</v>
@@ -8898,7 +8890,7 @@
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A166" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B166">
         <v>18.9712</v>
@@ -8946,7 +8938,7 @@
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A167" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B167">
         <v>18.9712</v>
@@ -8994,7 +8986,7 @@
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A168" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B168">
         <v>18.9712</v>
@@ -9043,7 +9035,7 @@
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A169" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B169">
         <v>18.9712</v>
@@ -9091,7 +9083,7 @@
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A170" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B170">
         <v>18.9712</v>
@@ -9139,7 +9131,7 @@
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A171" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B171">
         <v>18.1096</v>
@@ -9186,7 +9178,7 @@
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A172" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B172">
         <v>18.1096</v>
@@ -9233,7 +9225,7 @@
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A173" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B173">
         <v>18.1096</v>
@@ -9280,7 +9272,7 @@
     </row>
     <row r="174" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A174" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B174">
         <v>18.1096</v>
@@ -9327,7 +9319,7 @@
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A175" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B175">
         <v>18.1096</v>
@@ -9374,7 +9366,7 @@
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A176" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B176">
         <v>18.1096</v>
@@ -9421,7 +9413,7 @@
     </row>
     <row r="177" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A177" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B177">
         <v>18.1096</v>
@@ -9468,7 +9460,7 @@
     </row>
     <row r="178" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A178" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B178">
         <v>18.1096</v>
@@ -9515,7 +9507,7 @@
     </row>
     <row r="179" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A179" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B179">
         <v>18.1096</v>
@@ -9562,7 +9554,7 @@
     </row>
     <row r="180" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A180" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B180">
         <v>18.1096</v>
@@ -9609,7 +9601,7 @@
     </row>
     <row r="181" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A181" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B181">
         <v>18.1096</v>
@@ -9657,7 +9649,7 @@
     </row>
     <row r="182" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A182" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B182">
         <v>18.1096</v>
@@ -9705,7 +9697,7 @@
     </row>
     <row r="183" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A183" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B183">
         <v>18.1096</v>
@@ -9753,7 +9745,7 @@
     </row>
     <row r="184" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A184" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B184">
         <v>14.641500000000001</v>
@@ -9801,7 +9793,7 @@
     </row>
     <row r="185" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A185" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B185">
         <v>14.641500000000001</v>
@@ -9849,7 +9841,7 @@
     </row>
     <row r="186" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A186" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B186">
         <v>14.641500000000001</v>
@@ -9897,7 +9889,7 @@
     </row>
     <row r="187" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A187" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B187">
         <v>14.641500000000001</v>
@@ -9945,7 +9937,7 @@
     </row>
     <row r="188" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A188" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B188">
         <v>14.641500000000001</v>
@@ -9993,7 +9985,7 @@
     </row>
     <row r="189" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A189" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B189">
         <v>14.641500000000001</v>
@@ -10041,7 +10033,7 @@
     </row>
     <row r="190" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A190" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B190">
         <v>14.641500000000001</v>
@@ -10089,7 +10081,7 @@
     </row>
     <row r="191" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A191" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B191">
         <v>14.641500000000001</v>
@@ -10137,7 +10129,7 @@
     </row>
     <row r="192" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A192" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B192">
         <v>14.641500000000001</v>
@@ -10185,7 +10177,7 @@
     </row>
     <row r="193" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A193" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B193">
         <v>14.641500000000001</v>
@@ -10233,7 +10225,7 @@
     </row>
     <row r="194" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A194" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B194">
         <v>14.641500000000001</v>
@@ -10282,7 +10274,7 @@
     </row>
     <row r="195" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A195" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B195">
         <v>14.641500000000001</v>
@@ -10331,7 +10323,7 @@
     </row>
     <row r="196" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A196" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B196">
         <v>14.641500000000001</v>
@@ -10379,7 +10371,7 @@
     </row>
     <row r="197" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A197" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B197">
         <v>16.742498000000001</v>
@@ -10426,7 +10418,7 @@
     </row>
     <row r="198" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A198" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B198">
         <v>16.742498000000001</v>
@@ -10473,7 +10465,7 @@
     </row>
     <row r="199" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A199" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B199">
         <v>16.742498000000001</v>
@@ -10520,7 +10512,7 @@
     </row>
     <row r="200" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A200" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B200">
         <v>16.742498000000001</v>
@@ -10567,7 +10559,7 @@
     </row>
     <row r="201" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A201" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B201">
         <v>16.742498000000001</v>
@@ -10614,7 +10606,7 @@
     </row>
     <row r="202" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A202" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B202">
         <v>16.742498000000001</v>
@@ -10661,7 +10653,7 @@
     </row>
     <row r="203" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A203" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B203">
         <v>16.742498000000001</v>
@@ -10708,7 +10700,7 @@
     </row>
     <row r="204" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A204" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B204">
         <v>16.742498000000001</v>
@@ -10755,7 +10747,7 @@
     </row>
     <row r="205" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A205" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B205">
         <v>16.742498000000001</v>
@@ -10802,7 +10794,7 @@
     </row>
     <row r="206" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A206" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B206">
         <v>16.742498000000001</v>
@@ -10849,7 +10841,7 @@
     </row>
     <row r="207" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A207" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B207">
         <v>16.742498000000001</v>
@@ -10897,7 +10889,7 @@
     </row>
     <row r="208" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A208" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B208">
         <v>16.742498000000001</v>
@@ -10945,7 +10937,7 @@
     </row>
     <row r="209" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A209" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B209">
         <v>16.742498000000001</v>
@@ -10993,7 +10985,7 @@
     </row>
     <row r="210" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A210" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B210">
         <v>18.220800000000001</v>
@@ -11040,7 +11032,7 @@
     </row>
     <row r="211" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A211" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B211">
         <v>18.220800000000001</v>
@@ -11087,7 +11079,7 @@
     </row>
     <row r="212" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A212" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B212">
         <v>18.220800000000001</v>
@@ -11134,7 +11126,7 @@
     </row>
     <row r="213" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A213" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B213">
         <v>18.220800000000001</v>
@@ -11181,7 +11173,7 @@
     </row>
     <row r="214" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A214" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B214">
         <v>18.220800000000001</v>
@@ -11228,7 +11220,7 @@
     </row>
     <row r="215" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A215" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B215">
         <v>18.220800000000001</v>
@@ -11275,7 +11267,7 @@
     </row>
     <row r="216" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A216" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B216">
         <v>18.220800000000001</v>
@@ -11322,7 +11314,7 @@
     </row>
     <row r="217" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A217" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B217">
         <v>18.220800000000001</v>
@@ -11369,7 +11361,7 @@
     </row>
     <row r="218" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A218" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B218">
         <v>18.220800000000001</v>
@@ -11416,7 +11408,7 @@
     </row>
     <row r="219" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A219" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B219">
         <v>18.220800000000001</v>
@@ -11463,7 +11455,7 @@
     </row>
     <row r="220" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A220" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B220">
         <v>18.220800000000001</v>
@@ -11511,7 +11503,7 @@
     </row>
     <row r="221" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A221" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B221">
         <v>18.220800000000001</v>
@@ -11559,7 +11551,7 @@
     </row>
     <row r="222" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A222" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B222">
         <v>18.220800000000001</v>
@@ -11607,7 +11599,7 @@
     </row>
     <row r="223" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A223" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B223">
         <v>17.357821999999999</v>
@@ -11654,7 +11646,7 @@
     </row>
     <row r="224" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A224" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B224">
         <v>17.357821999999999</v>
@@ -11701,7 +11693,7 @@
     </row>
     <row r="225" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A225" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B225">
         <v>17.357821999999999</v>
@@ -11748,7 +11740,7 @@
     </row>
     <row r="226" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A226" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B226">
         <v>17.357821999999999</v>
@@ -11795,7 +11787,7 @@
     </row>
     <row r="227" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A227" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B227">
         <v>17.357821999999999</v>
@@ -11842,7 +11834,7 @@
     </row>
     <row r="228" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A228" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B228">
         <v>17.357821999999999</v>
@@ -11889,7 +11881,7 @@
     </row>
     <row r="229" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A229" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B229">
         <v>17.357821999999999</v>
@@ -11936,7 +11928,7 @@
     </row>
     <row r="230" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A230" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B230">
         <v>17.357821999999999</v>
@@ -11983,7 +11975,7 @@
     </row>
     <row r="231" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A231" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B231">
         <v>17.357821999999999</v>
@@ -12030,7 +12022,7 @@
     </row>
     <row r="232" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A232" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B232">
         <v>17.357821999999999</v>
@@ -12077,7 +12069,7 @@
     </row>
     <row r="233" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A233" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B233">
         <v>17.357821999999999</v>
@@ -12125,7 +12117,7 @@
     </row>
     <row r="234" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A234" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B234">
         <v>17.357821999999999</v>
@@ -12173,7 +12165,7 @@
     </row>
     <row r="235" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A235" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B235">
         <v>17.357821999999999</v>
@@ -12221,7 +12213,7 @@
     </row>
     <row r="236" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A236" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B236">
         <v>13.9094</v>
@@ -12268,7 +12260,7 @@
     </row>
     <row r="237" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A237" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B237">
         <v>13.9094</v>
@@ -12315,7 +12307,7 @@
     </row>
     <row r="238" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A238" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B238">
         <v>13.9094</v>
@@ -12362,7 +12354,7 @@
     </row>
     <row r="239" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A239" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B239">
         <v>13.9094</v>
@@ -12409,7 +12401,7 @@
     </row>
     <row r="240" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A240" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B240">
         <v>13.9094</v>
@@ -12456,7 +12448,7 @@
     </row>
     <row r="241" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A241" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B241">
         <v>13.9094</v>
@@ -12503,7 +12495,7 @@
     </row>
     <row r="242" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A242" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B242">
         <v>13.9094</v>
@@ -12550,7 +12542,7 @@
     </row>
     <row r="243" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A243" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B243">
         <v>13.9094</v>
@@ -12597,7 +12589,7 @@
     </row>
     <row r="244" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A244" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B244">
         <v>13.9094</v>
@@ -12644,7 +12636,7 @@
     </row>
     <row r="245" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A245" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B245">
         <v>13.9094</v>
@@ -12691,7 +12683,7 @@
     </row>
     <row r="246" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A246" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B246">
         <v>13.9094</v>
@@ -12739,7 +12731,7 @@
     </row>
     <row r="247" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A247" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B247">
         <v>13.9094</v>
@@ -12787,7 +12779,7 @@
     </row>
     <row r="248" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A248" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B248">
         <v>13.9094</v>
@@ -12835,7 +12827,7 @@
     </row>
     <row r="249" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A249" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B249">
         <v>12.984299999999999</v>
@@ -12882,7 +12874,7 @@
     </row>
     <row r="250" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A250" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B250">
         <v>12.984299999999999</v>
@@ -12929,7 +12921,7 @@
     </row>
     <row r="251" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A251" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B251">
         <v>12.984299999999999</v>
@@ -12976,7 +12968,7 @@
     </row>
     <row r="252" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A252" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B252">
         <v>12.984299999999999</v>
@@ -13023,7 +13015,7 @@
     </row>
     <row r="253" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A253" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B253">
         <v>12.984299999999999</v>
@@ -13070,7 +13062,7 @@
     </row>
     <row r="254" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A254" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B254">
         <v>12.984299999999999</v>
@@ -13117,7 +13109,7 @@
     </row>
     <row r="255" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A255" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B255">
         <v>12.984299999999999</v>
@@ -13164,7 +13156,7 @@
     </row>
     <row r="256" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A256" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B256">
         <v>12.984299999999999</v>
@@ -13211,7 +13203,7 @@
     </row>
     <row r="257" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A257" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B257">
         <v>12.984299999999999</v>
@@ -13258,7 +13250,7 @@
     </row>
     <row r="258" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A258" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B258">
         <v>12.984299999999999</v>
@@ -13305,7 +13297,7 @@
     </row>
     <row r="259" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A259" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B259">
         <v>12.984299999999999</v>
@@ -13353,7 +13345,7 @@
     </row>
     <row r="260" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A260" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B260">
         <v>12.984299999999999</v>
@@ -13401,7 +13393,7 @@
     </row>
     <row r="261" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A261" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B261">
         <v>12.984299999999999</v>
@@ -13449,7 +13441,7 @@
     </row>
     <row r="262" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A262" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B262">
         <v>18.0425</v>
@@ -13496,7 +13488,7 @@
     </row>
     <row r="263" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A263" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B263">
         <v>18.0425</v>
@@ -13543,7 +13535,7 @@
     </row>
     <row r="264" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A264" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B264">
         <v>18.0425</v>
@@ -13590,7 +13582,7 @@
     </row>
     <row r="265" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A265" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B265">
         <v>18.0425</v>
@@ -13637,7 +13629,7 @@
     </row>
     <row r="266" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A266" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B266">
         <v>18.0425</v>
@@ -13684,7 +13676,7 @@
     </row>
     <row r="267" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A267" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B267">
         <v>18.0425</v>
@@ -13731,7 +13723,7 @@
     </row>
     <row r="268" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A268" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B268">
         <v>18.0425</v>
@@ -13778,7 +13770,7 @@
     </row>
     <row r="269" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A269" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B269">
         <v>18.0425</v>
@@ -13825,7 +13817,7 @@
     </row>
     <row r="270" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A270" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B270">
         <v>18.0425</v>
@@ -13872,7 +13864,7 @@
     </row>
     <row r="271" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A271" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B271">
         <v>18.0425</v>
@@ -13919,7 +13911,7 @@
     </row>
     <row r="272" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A272" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B272">
         <v>18.0425</v>
@@ -13967,7 +13959,7 @@
     </row>
     <row r="273" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A273" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B273">
         <v>18.0425</v>
@@ -14015,7 +14007,7 @@
     </row>
     <row r="274" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A274" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B274">
         <v>18.0425</v>
@@ -14063,7 +14055,7 @@
     </row>
     <row r="275" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A275" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B275">
         <v>10.691800000000001</v>
@@ -14112,7 +14104,7 @@
     </row>
     <row r="276" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A276" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B276">
         <v>10.691800000000001</v>
@@ -14161,7 +14153,7 @@
     </row>
     <row r="277" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A277" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B277">
         <v>10.691800000000001</v>
@@ -14210,7 +14202,7 @@
     </row>
     <row r="278" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A278" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B278">
         <v>10.691800000000001</v>
@@ -14259,7 +14251,7 @@
     </row>
     <row r="279" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A279" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B279">
         <v>10.691800000000001</v>
@@ -14308,7 +14300,7 @@
     </row>
     <row r="280" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A280" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B280">
         <v>10.691800000000001</v>
@@ -14357,7 +14349,7 @@
     </row>
     <row r="281" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A281" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B281">
         <v>10.691800000000001</v>
@@ -14406,7 +14398,7 @@
     </row>
     <row r="282" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A282" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B282">
         <v>10.691800000000001</v>
@@ -14455,7 +14447,7 @@
     </row>
     <row r="283" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A283" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B283">
         <v>10.691800000000001</v>
@@ -14504,7 +14496,7 @@
     </row>
     <row r="284" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A284" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B284">
         <v>10.691800000000001</v>
@@ -14553,7 +14545,7 @@
     </row>
     <row r="285" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A285" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B285">
         <v>10.691800000000001</v>
@@ -14603,7 +14595,7 @@
     </row>
     <row r="286" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A286" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B286">
         <v>10.691800000000001</v>
@@ -14652,7 +14644,7 @@
     </row>
     <row r="287" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A287" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B287">
         <v>10.691800000000001</v>
@@ -14700,7 +14692,7 @@
     </row>
     <row r="288" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A288" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B288">
         <v>21.693999999999999</v>
@@ -14747,7 +14739,7 @@
     </row>
     <row r="289" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A289" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B289">
         <v>21.693999999999999</v>
@@ -14794,7 +14786,7 @@
     </row>
     <row r="290" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A290" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B290">
         <v>21.693999999999999</v>
@@ -14841,7 +14833,7 @@
     </row>
     <row r="291" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A291" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B291">
         <v>21.693999999999999</v>
@@ -14888,7 +14880,7 @@
     </row>
     <row r="292" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A292" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B292">
         <v>21.693999999999999</v>
@@ -14935,7 +14927,7 @@
     </row>
     <row r="293" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A293" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B293">
         <v>21.693999999999999</v>
@@ -14982,7 +14974,7 @@
     </row>
     <row r="294" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A294" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B294">
         <v>21.693999999999999</v>
@@ -15029,7 +15021,7 @@
     </row>
     <row r="295" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A295" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B295">
         <v>21.693999999999999</v>
@@ -15076,7 +15068,7 @@
     </row>
     <row r="296" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A296" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B296">
         <v>21.693999999999999</v>
@@ -15123,7 +15115,7 @@
     </row>
     <row r="297" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A297" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B297">
         <v>21.693999999999999</v>
@@ -15170,7 +15162,7 @@
     </row>
     <row r="298" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A298" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B298">
         <v>21.693999999999999</v>
@@ -15218,7 +15210,7 @@
     </row>
     <row r="299" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A299" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B299">
         <v>21.693999999999999</v>
@@ -15266,7 +15258,7 @@
     </row>
     <row r="300" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A300" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B300">
         <v>21.693999999999999</v>
@@ -15314,7 +15306,7 @@
     </row>
     <row r="301" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A301" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B301">
         <v>18.335799999999999</v>
@@ -15361,7 +15353,7 @@
     </row>
     <row r="302" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A302" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B302">
         <v>18.335799999999999</v>
@@ -15408,7 +15400,7 @@
     </row>
     <row r="303" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A303" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B303">
         <v>18.335799999999999</v>
@@ -15455,7 +15447,7 @@
     </row>
     <row r="304" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A304" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B304">
         <v>18.335799999999999</v>
@@ -15502,7 +15494,7 @@
     </row>
     <row r="305" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A305" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B305">
         <v>18.335799999999999</v>
@@ -15549,7 +15541,7 @@
     </row>
     <row r="306" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A306" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B306">
         <v>18.335799999999999</v>
@@ -15596,7 +15588,7 @@
     </row>
     <row r="307" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A307" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B307">
         <v>18.335799999999999</v>
@@ -15643,7 +15635,7 @@
     </row>
     <row r="308" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A308" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B308">
         <v>18.335799999999999</v>
@@ -15690,7 +15682,7 @@
     </row>
     <row r="309" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A309" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B309">
         <v>18.335799999999999</v>
@@ -15737,7 +15729,7 @@
     </row>
     <row r="310" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A310" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B310">
         <v>18.335799999999999</v>
@@ -15784,7 +15776,7 @@
     </row>
     <row r="311" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A311" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B311">
         <v>18.335799999999999</v>
@@ -15832,7 +15824,7 @@
     </row>
     <row r="312" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A312" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B312">
         <v>18.335799999999999</v>
@@ -15880,7 +15872,7 @@
     </row>
     <row r="313" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A313" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B313">
         <v>18.335799999999999</v>
@@ -15925,1549 +15917,6 @@
         <f t="shared" si="14"/>
         <v>2.688742659024977E-3</v>
       </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526EAC78-B7AA-FC48-A460-9EAC72D4A554}">
-  <dimension ref="A1:H105"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="32.5" customWidth="1"/>
-    <col min="5" max="8" width="21.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C2">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D2" s="21">
-        <v>43466</v>
-      </c>
-      <c r="E2" s="12">
-        <v>489600</v>
-      </c>
-      <c r="F2" s="12">
-        <v>0</v>
-      </c>
-      <c r="G2" s="12">
-        <v>0</v>
-      </c>
-      <c r="H2" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B3">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C3">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D3" s="21">
-        <v>43497</v>
-      </c>
-      <c r="E3" s="12">
-        <v>459400</v>
-      </c>
-      <c r="F3" s="12">
-        <v>0</v>
-      </c>
-      <c r="G3" s="12">
-        <v>0</v>
-      </c>
-      <c r="H3" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C4">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D4" s="21">
-        <v>43525</v>
-      </c>
-      <c r="E4" s="12">
-        <v>521400</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0</v>
-      </c>
-      <c r="H4" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C5">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D5" s="21">
-        <v>43556</v>
-      </c>
-      <c r="E5" s="12">
-        <v>458100</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-      <c r="H5" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C6">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D6" s="21">
-        <v>43586</v>
-      </c>
-      <c r="E6" s="12">
-        <v>358300</v>
-      </c>
-      <c r="F6" s="12">
-        <v>0</v>
-      </c>
-      <c r="G6" s="12">
-        <v>0</v>
-      </c>
-      <c r="H6" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C7">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D7" s="21">
-        <v>43617</v>
-      </c>
-      <c r="E7" s="12">
-        <v>274800</v>
-      </c>
-      <c r="F7" s="12">
-        <v>0</v>
-      </c>
-      <c r="G7" s="12">
-        <v>0</v>
-      </c>
-      <c r="H7" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C8">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D8" s="21">
-        <v>43647</v>
-      </c>
-      <c r="E8" s="12">
-        <v>295000</v>
-      </c>
-      <c r="F8" s="12">
-        <v>0</v>
-      </c>
-      <c r="G8" s="12">
-        <v>0</v>
-      </c>
-      <c r="H8" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C9">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D9" s="21">
-        <v>43678</v>
-      </c>
-      <c r="E9" s="12">
-        <v>269300</v>
-      </c>
-      <c r="F9" s="12">
-        <v>0</v>
-      </c>
-      <c r="G9" s="12">
-        <v>0</v>
-      </c>
-      <c r="H9" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B10">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C10">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D10" s="21">
-        <v>43709</v>
-      </c>
-      <c r="E10" s="12">
-        <v>201300</v>
-      </c>
-      <c r="F10" s="12">
-        <v>0</v>
-      </c>
-      <c r="G10" s="12">
-        <v>0</v>
-      </c>
-      <c r="H10" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C11">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D11" s="21">
-        <v>43739</v>
-      </c>
-      <c r="E11" s="12">
-        <v>235600</v>
-      </c>
-      <c r="F11" s="12">
-        <v>0</v>
-      </c>
-      <c r="G11" s="12">
-        <v>0</v>
-      </c>
-      <c r="H11" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C12">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D12" s="21">
-        <v>43770</v>
-      </c>
-      <c r="E12" s="12">
-        <v>333900</v>
-      </c>
-      <c r="F12" s="12">
-        <v>0</v>
-      </c>
-      <c r="G12" s="12">
-        <v>0</v>
-      </c>
-      <c r="H12" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C13">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D13" s="21">
-        <v>43800</v>
-      </c>
-      <c r="E13" s="12">
-        <v>378700</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B14">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C14">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D14" s="21">
-        <v>43831</v>
-      </c>
-      <c r="E14" s="12">
-        <v>393700</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C15">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D15" s="21">
-        <v>43862</v>
-      </c>
-      <c r="E15" s="12">
-        <v>398900</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15" s="10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C16">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D16" s="21">
-        <v>43891</v>
-      </c>
-      <c r="E16" s="12">
-        <v>189400</v>
-      </c>
-      <c r="F16">
-        <v>186</v>
-      </c>
-      <c r="G16">
-        <v>6</v>
-      </c>
-      <c r="H16">
-        <f>G16/F16</f>
-        <v>3.2258064516129031E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C17">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D17" s="21">
-        <v>43922</v>
-      </c>
-      <c r="E17" s="12">
-        <v>1200</v>
-      </c>
-      <c r="F17">
-        <v>1315</v>
-      </c>
-      <c r="G17">
-        <v>55</v>
-      </c>
-      <c r="H17">
-        <f t="shared" ref="H17:H49" si="0">G17/F17</f>
-        <v>4.1825095057034217E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C18">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D18" s="21">
-        <v>43952</v>
-      </c>
-      <c r="E18" s="12">
-        <v>1000</v>
-      </c>
-      <c r="F18">
-        <v>544</v>
-      </c>
-      <c r="G18">
-        <v>22</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="0"/>
-        <v>4.0441176470588237E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B19">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C19">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D19" s="21">
-        <v>43983</v>
-      </c>
-      <c r="E19" s="12">
-        <v>1100</v>
-      </c>
-      <c r="F19">
-        <v>296</v>
-      </c>
-      <c r="G19">
-        <v>3</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="0"/>
-        <v>1.0135135135135136E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B20">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C20">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D20" s="21">
-        <v>44013</v>
-      </c>
-      <c r="E20" s="12">
-        <v>1500</v>
-      </c>
-      <c r="F20">
-        <v>267</v>
-      </c>
-      <c r="G20">
-        <v>1</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="0"/>
-        <v>3.7453183520599251E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C21">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D21" s="21">
-        <v>44044</v>
-      </c>
-      <c r="E21" s="12">
-        <v>1300</v>
-      </c>
-      <c r="F21">
-        <v>1424</v>
-      </c>
-      <c r="G21">
-        <v>7</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="0"/>
-        <v>4.9157303370786515E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C22">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D22" s="21">
-        <v>44075</v>
-      </c>
-      <c r="E22" s="12">
-        <v>1700</v>
-      </c>
-      <c r="F22">
-        <v>1565</v>
-      </c>
-      <c r="G22">
-        <v>28</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="0"/>
-        <v>1.7891373801916934E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C23">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D23" s="21">
-        <v>44105</v>
-      </c>
-      <c r="E23" s="12">
-        <v>3300</v>
-      </c>
-      <c r="F23">
-        <v>1290</v>
-      </c>
-      <c r="G23">
-        <v>6</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="0"/>
-        <v>4.6511627906976744E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B24">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C24">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D24" s="21">
-        <v>44136</v>
-      </c>
-      <c r="E24" s="12">
-        <v>28000</v>
-      </c>
-      <c r="F24">
-        <v>1397</v>
-      </c>
-      <c r="G24">
-        <v>7</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="0"/>
-        <v>5.0107372942018611E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C25">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D25" s="21">
-        <v>44166</v>
-      </c>
-      <c r="E25" s="12">
-        <v>64900.000000000007</v>
-      </c>
-      <c r="F25">
-        <v>3579</v>
-      </c>
-      <c r="G25">
-        <v>11</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="0"/>
-        <v>3.073484213467449E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B26">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C26">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D26" s="21">
-        <v>44197</v>
-      </c>
-      <c r="E26" s="12">
-        <v>22300</v>
-      </c>
-      <c r="F26">
-        <v>14823</v>
-      </c>
-      <c r="G26">
-        <v>68</v>
-      </c>
-      <c r="H26">
-        <f t="shared" si="0"/>
-        <v>4.5874654253524926E-3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C27">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D27" s="21">
-        <v>44228</v>
-      </c>
-      <c r="E27" s="12">
-        <v>13200</v>
-      </c>
-      <c r="F27">
-        <v>23093</v>
-      </c>
-      <c r="G27">
-        <v>108</v>
-      </c>
-      <c r="H27">
-        <f t="shared" si="0"/>
-        <v>4.6767418698306848E-3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C28">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D28" s="21">
-        <v>44256</v>
-      </c>
-      <c r="E28" s="12">
-        <v>12500</v>
-      </c>
-      <c r="F28">
-        <v>25484</v>
-      </c>
-      <c r="G28">
-        <v>102</v>
-      </c>
-      <c r="H28">
-        <f t="shared" si="0"/>
-        <v>4.002511379689217E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C29">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D29" s="21">
-        <v>44287</v>
-      </c>
-      <c r="E29" s="12">
-        <v>16600</v>
-      </c>
-      <c r="F29">
-        <v>31444</v>
-      </c>
-      <c r="G29">
-        <v>220</v>
-      </c>
-      <c r="H29">
-        <f t="shared" si="0"/>
-        <v>6.9965653224780561E-3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B30">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C30">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D30" s="21">
-        <v>44317</v>
-      </c>
-      <c r="E30" s="12">
-        <v>23500</v>
-      </c>
-      <c r="F30">
-        <v>35559</v>
-      </c>
-      <c r="G30">
-        <v>314</v>
-      </c>
-      <c r="H30">
-        <f t="shared" si="0"/>
-        <v>8.8303945555274332E-3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B31">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C31">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D31" s="21">
-        <v>44348</v>
-      </c>
-      <c r="E31" s="12">
-        <v>26200</v>
-      </c>
-      <c r="F31">
-        <v>48727</v>
-      </c>
-      <c r="G31">
-        <v>326</v>
-      </c>
-      <c r="H31">
-        <f t="shared" si="0"/>
-        <v>6.6903359533728732E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C32">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D32" s="21">
-        <v>44378</v>
-      </c>
-      <c r="E32" s="12">
-        <v>26900</v>
-      </c>
-      <c r="F32">
-        <v>193603</v>
-      </c>
-      <c r="G32">
-        <v>1474</v>
-      </c>
-      <c r="H32">
-        <f t="shared" si="0"/>
-        <v>7.6135183855622068E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C33">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D33" s="21">
-        <v>44409</v>
-      </c>
-      <c r="E33" s="12">
-        <v>22400</v>
-      </c>
-      <c r="F33">
-        <v>268259</v>
-      </c>
-      <c r="G33">
-        <v>2545</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="0"/>
-        <v>9.4871001532101443E-3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B34">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C34">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D34" s="21">
-        <v>44440</v>
-      </c>
-      <c r="E34" s="12">
-        <v>17000</v>
-      </c>
-      <c r="F34">
-        <v>224573</v>
-      </c>
-      <c r="G34">
-        <v>2133</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="0"/>
-        <v>9.4980251410454498E-3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B35">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C35">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D35" s="21">
-        <v>44470</v>
-      </c>
-      <c r="E35" s="12">
-        <v>23200</v>
-      </c>
-      <c r="F35">
-        <v>74573</v>
-      </c>
-      <c r="G35">
-        <v>800</v>
-      </c>
-      <c r="H35">
-        <f t="shared" si="0"/>
-        <v>1.0727743285103187E-2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B36">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C36">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D36" s="21">
-        <v>44501</v>
-      </c>
-      <c r="E36" s="12">
-        <v>51100</v>
-      </c>
-      <c r="F36">
-        <v>10485</v>
-      </c>
-      <c r="G36">
-        <v>68</v>
-      </c>
-      <c r="H36">
-        <f t="shared" si="0"/>
-        <v>6.4854554124940391E-3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B37">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C37">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D37" s="21">
-        <v>44531</v>
-      </c>
-      <c r="E37" s="12">
-        <v>101300</v>
-      </c>
-      <c r="F37">
-        <v>3518</v>
-      </c>
-      <c r="G37">
-        <v>18</v>
-      </c>
-      <c r="H37">
-        <f t="shared" si="0"/>
-        <v>5.1165434906196702E-3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B38">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C38">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D38" s="21">
-        <v>44562</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38">
-        <v>78786</v>
-      </c>
-      <c r="G38">
-        <v>77</v>
-      </c>
-      <c r="H38">
-        <f t="shared" si="0"/>
-        <v>9.7733099789302667E-4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C39">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D39" s="21">
-        <v>44593</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F39">
-        <v>25072</v>
-      </c>
-      <c r="G39">
-        <v>95</v>
-      </c>
-      <c r="H39">
-        <f t="shared" si="0"/>
-        <v>3.7890874282067643E-3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B40">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C40">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D40" s="21">
-        <v>44621</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F40">
-        <v>20423</v>
-      </c>
-      <c r="G40">
-        <v>16</v>
-      </c>
-      <c r="H40">
-        <f t="shared" si="0"/>
-        <v>7.8343044606571019E-4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B41">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C41">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D41" s="21">
-        <v>44652</v>
-      </c>
-      <c r="E41" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F41">
-        <v>12656</v>
-      </c>
-      <c r="G41">
-        <v>16</v>
-      </c>
-      <c r="H41">
-        <f t="shared" si="0"/>
-        <v>1.2642225031605564E-3</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B42">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C42">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D42" s="21">
-        <v>44682</v>
-      </c>
-      <c r="E42" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F42">
-        <v>2378</v>
-      </c>
-      <c r="G42">
-        <v>3</v>
-      </c>
-      <c r="H42">
-        <f t="shared" si="0"/>
-        <v>1.2615643397813289E-3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C43">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D43" s="21">
-        <v>44713</v>
-      </c>
-      <c r="E43" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F43">
-        <v>704</v>
-      </c>
-      <c r="G43">
-        <v>0</v>
-      </c>
-      <c r="H43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B44">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C44">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D44" s="21">
-        <v>44743</v>
-      </c>
-      <c r="E44" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F44">
-        <v>2071</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B45">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C45">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D45" s="21">
-        <v>44774</v>
-      </c>
-      <c r="E45" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F45">
-        <v>2445</v>
-      </c>
-      <c r="G45">
-        <v>1</v>
-      </c>
-      <c r="H45">
-        <f t="shared" si="0"/>
-        <v>4.0899795501022495E-4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C46">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D46" s="21">
-        <v>44805</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F46">
-        <v>647</v>
-      </c>
-      <c r="G46">
-        <v>0</v>
-      </c>
-      <c r="H46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B47">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C47">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D47" s="21">
-        <v>44835</v>
-      </c>
-      <c r="E47" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F47">
-        <v>99</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B48">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C48">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D48" s="21">
-        <v>44866</v>
-      </c>
-      <c r="E48" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F48">
-        <v>107</v>
-      </c>
-      <c r="G48">
-        <v>0</v>
-      </c>
-      <c r="H48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="B49">
-        <v>21.521757000000001</v>
-      </c>
-      <c r="C49">
-        <v>-77.781166999999996</v>
-      </c>
-      <c r="D49" s="21">
-        <v>44896</v>
-      </c>
-      <c r="E49" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F49">
-        <v>601</v>
-      </c>
-      <c r="G49">
-        <v>0</v>
-      </c>
-      <c r="H49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="11"/>
-      <c r="D50" s="21"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="11"/>
-      <c r="D51" s="21"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="11"/>
-      <c r="D52" s="21"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="11"/>
-      <c r="D53" s="21"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="11"/>
-      <c r="D54" s="21"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="11"/>
-      <c r="D55" s="21"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="11"/>
-      <c r="D56" s="21"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="11"/>
-      <c r="D57" s="21"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="11"/>
-      <c r="D58" s="21"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="11"/>
-      <c r="D59" s="21"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="11"/>
-      <c r="D60" s="21"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="11"/>
-      <c r="D61" s="21"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A62" s="11"/>
-      <c r="D62" s="21"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="11"/>
-      <c r="D63" s="21"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="11"/>
-      <c r="D64" s="21"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="11"/>
-      <c r="D65" s="21"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A66" s="11"/>
-      <c r="D66" s="21"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="11"/>
-      <c r="D67" s="21"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="11"/>
-      <c r="D68" s="21"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="11"/>
-      <c r="D69" s="21"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A70" s="11"/>
-      <c r="D70" s="21"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="11"/>
-      <c r="D71" s="21"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="11"/>
-      <c r="D72" s="21"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="11"/>
-      <c r="D73" s="21"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="11"/>
-      <c r="D74" s="21"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A75" s="11"/>
-      <c r="D75" s="21"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="11"/>
-      <c r="D76" s="21"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A77" s="11"/>
-      <c r="D77" s="21"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A78" s="11"/>
-      <c r="D78" s="21"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A79" s="11"/>
-      <c r="D79" s="21"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A80" s="11"/>
-      <c r="D80" s="21"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A81" s="11"/>
-      <c r="D81" s="21"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" s="11"/>
-      <c r="D82" s="21"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A83" s="11"/>
-      <c r="D83" s="21"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A84" s="11"/>
-      <c r="D84" s="21"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A85" s="11"/>
-      <c r="D85" s="21"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A86" s="11"/>
-      <c r="D86" s="21"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A87" s="11"/>
-      <c r="D87" s="21"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A88" s="11"/>
-      <c r="D88" s="21"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A89" s="11"/>
-      <c r="D89" s="21"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A90" s="11"/>
-      <c r="D90" s="21"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A91" s="11"/>
-      <c r="D91" s="21"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A92" s="11"/>
-      <c r="D92" s="21"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A93" s="11"/>
-      <c r="D93" s="21"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A94" s="11"/>
-      <c r="D94" s="21"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A95" s="11"/>
-      <c r="D95" s="21"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A96" s="11"/>
-      <c r="D96" s="21"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A97" s="11"/>
-      <c r="D97" s="21"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A98" s="11"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A99" s="11"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A100" s="11"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A101" s="11"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A102" s="11"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A103" s="11"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A104" s="11"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A105" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>